<commit_message>
- Update ChangeRegionHead Extension table and fix Extension form constraints - Fix SyncFilesService export of region heads
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/extension-forms/xls/change_region_head_ext.xlsx
+++ b/src/main/resources/samples/extension-forms/xls/change_region_head_ext.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>type</t>
   </si>
@@ -219,7 +219,7 @@
     <t>version</t>
   </si>
   <si>
-    <t>HDS Change Head of Household Extension</t>
+    <t>HDS Change Head of Region Extension</t>
   </si>
   <si>
     <t>change_region_head_ext</t>
@@ -236,10 +236,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -284,6 +284,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -292,33 +308,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -338,14 +348,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,23 +377,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,31 +407,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -422,7 +415,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,19 +449,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,37 +473,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,7 +497,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,7 +521,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +557,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,79 +629,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,10 +643,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -670,8 +705,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,198 +740,163 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -926,14 +926,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -967,9 +959,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1378,243 +1367,243 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="A8:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="27.3666666666667" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.6333333333333" style="19" customWidth="1"/>
-    <col min="3" max="3" width="29.1833333333333" style="19" customWidth="1"/>
-    <col min="4" max="4" width="29.375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="42.6" style="19" customWidth="1"/>
-    <col min="6" max="6" width="27.9083333333333" style="19" customWidth="1"/>
-    <col min="7" max="7" width="9" style="19"/>
-    <col min="8" max="8" width="21.625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="24.5" style="19" customWidth="1"/>
+    <col min="1" max="1" width="27.3666666666667" style="15" customWidth="1"/>
+    <col min="2" max="2" width="18.6333333333333" style="15" customWidth="1"/>
+    <col min="3" max="3" width="29.1833333333333" style="15" customWidth="1"/>
+    <col min="4" max="4" width="29.375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="42.6" style="15" customWidth="1"/>
+    <col min="6" max="6" width="27.9083333333333" style="15" customWidth="1"/>
+    <col min="7" max="7" width="9" style="15"/>
+    <col min="8" max="8" width="21.625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="24.5" style="15" customWidth="1"/>
     <col min="10" max="10" width="9" style="6"/>
-    <col min="11" max="11" width="30.9083333333333" style="19" customWidth="1"/>
-    <col min="12" max="13" width="9" style="19"/>
+    <col min="11" max="11" width="30.9083333333333" style="15" customWidth="1"/>
+    <col min="12" max="13" width="9" style="15"/>
     <col min="14" max="14" width="9" style="6"/>
-    <col min="15" max="15" width="9" style="19"/>
-    <col min="16" max="16" width="10.75" style="19" customWidth="1"/>
-    <col min="17" max="17" width="11.5" style="19" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="19"/>
+    <col min="15" max="15" width="9" style="15"/>
+    <col min="16" max="16" width="10.75" style="15" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="15" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A1" s="31" t="s">
+    <row r="1" s="9" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" s="28" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A2" s="33" t="s">
+    <row r="2" s="23" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="39" t="s">
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-    </row>
-    <row r="3" s="28" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A3" s="33" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+    </row>
+    <row r="3" s="23" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="39" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-    </row>
-    <row r="4" s="28" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
-      <c r="A4" s="33" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+    </row>
+    <row r="4" s="23" customFormat="1" ht="16.5" customHeight="1" spans="1:22">
+      <c r="A4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="39" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-    </row>
-    <row r="5" s="29" customFormat="1" spans="1:14">
-      <c r="A5" s="29" t="s">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+    </row>
+    <row r="5" s="24" customFormat="1" spans="1:14">
+      <c r="A5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="N5" s="35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" s="29" customFormat="1" spans="1:14">
-      <c r="A6" s="29" t="s">
+    <row r="6" s="24" customFormat="1" spans="1:14">
+      <c r="A6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="N6" s="40" t="s">
+      <c r="J6" s="35"/>
+      <c r="N6" s="35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" s="29" customFormat="1" spans="1:14">
-      <c r="A7" s="29" t="s">
+    <row r="7" s="24" customFormat="1" spans="1:14">
+      <c r="A7" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1623,18 +1612,18 @@
       <c r="D7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" s="29" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A8" s="29" t="s">
+    <row r="8" s="24" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1643,18 +1632,16 @@
       <c r="D8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="35"/>
+      <c r="N8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" s="29" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A9" s="29" t="s">
+    </row>
+    <row r="9" s="24" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1663,18 +1650,16 @@
       <c r="D9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="35"/>
+      <c r="N9" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" s="29" customFormat="1" spans="1:14">
-      <c r="A10" s="29" t="s">
+    </row>
+    <row r="10" s="24" customFormat="1" spans="1:14">
+      <c r="A10" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1683,18 +1668,18 @@
       <c r="D10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="40" t="s">
+      <c r="N10" s="35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" s="29" customFormat="1" spans="1:14">
-      <c r="A11" s="29" t="s">
+    <row r="11" s="24" customFormat="1" spans="1:14">
+      <c r="A11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="24" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -1703,225 +1688,225 @@
       <c r="D11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="40" t="s">
+      <c r="J11" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="40" t="s">
+      <c r="N11" s="35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" s="30" customFormat="1" spans="1:14">
-      <c r="A12" s="30" t="s">
+    <row r="12" s="25" customFormat="1" spans="1:14">
+      <c r="A12" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="41"/>
-      <c r="N12" s="41"/>
-    </row>
-    <row r="13" s="30" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A13" s="30" t="s">
+      <c r="J12" s="36"/>
+      <c r="N12" s="36"/>
+    </row>
+    <row r="13" s="25" customFormat="1" customHeight="1" spans="1:14">
+      <c r="A13" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="J13" s="41"/>
-      <c r="N13" s="41"/>
-    </row>
-    <row r="14" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J14" s="40"/>
-      <c r="N14" s="40"/>
-    </row>
-    <row r="15" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J15" s="40"/>
-      <c r="N15" s="40"/>
-    </row>
-    <row r="16" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J16" s="40"/>
-      <c r="N16" s="40"/>
-    </row>
-    <row r="17" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J17" s="40"/>
-      <c r="N17" s="40"/>
-    </row>
-    <row r="18" s="29" customFormat="1" spans="10:14">
-      <c r="J18" s="40"/>
-      <c r="N18" s="40"/>
-    </row>
-    <row r="19" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J19" s="40"/>
-      <c r="N19" s="40"/>
-    </row>
-    <row r="20" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J20" s="40"/>
-      <c r="N20" s="40"/>
-    </row>
-    <row r="21" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J21" s="40"/>
-      <c r="N21" s="40"/>
-    </row>
-    <row r="22" s="29" customFormat="1" spans="10:14">
-      <c r="J22" s="40"/>
-      <c r="N22" s="40"/>
-    </row>
-    <row r="23" s="29" customFormat="1" spans="10:14">
-      <c r="J23" s="40"/>
-      <c r="N23" s="40"/>
-    </row>
-    <row r="24" s="29" customFormat="1" spans="10:14">
-      <c r="J24" s="40"/>
-      <c r="N24" s="40"/>
-    </row>
-    <row r="25" s="29" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
-      <c r="J25" s="40"/>
-      <c r="N25" s="40"/>
-    </row>
-    <row r="26" s="29" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J26" s="40"/>
-      <c r="N26" s="40"/>
-    </row>
-    <row r="27" s="29" customFormat="1" spans="10:14">
-      <c r="J27" s="40"/>
-      <c r="N27" s="40"/>
-    </row>
-    <row r="28" s="29" customFormat="1" spans="10:14">
-      <c r="J28" s="40"/>
-      <c r="N28" s="40"/>
-    </row>
-    <row r="29" s="29" customFormat="1" spans="10:14">
-      <c r="J29" s="40"/>
-      <c r="N29" s="40"/>
-    </row>
-    <row r="30" s="29" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
-      <c r="J30" s="40"/>
-      <c r="N30" s="40"/>
-    </row>
-    <row r="31" s="29" customFormat="1" spans="10:14">
-      <c r="J31" s="40"/>
-      <c r="N31" s="40"/>
-    </row>
-    <row r="32" s="29" customFormat="1" spans="10:14">
-      <c r="J32" s="40"/>
-      <c r="N32" s="40"/>
-    </row>
-    <row r="33" s="29" customFormat="1" spans="10:14">
-      <c r="J33" s="40"/>
-      <c r="N33" s="40"/>
-    </row>
-    <row r="34" s="29" customFormat="1" spans="10:14">
-      <c r="J34" s="40"/>
-      <c r="N34" s="40"/>
-    </row>
-    <row r="35" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J35" s="40"/>
-      <c r="N35" s="40"/>
-    </row>
-    <row r="36" s="29" customFormat="1" ht="12" customHeight="1" spans="10:14">
-      <c r="J36" s="40"/>
-      <c r="N36" s="40"/>
-    </row>
-    <row r="37" s="29" customFormat="1" spans="10:14">
-      <c r="J37" s="40"/>
-      <c r="N37" s="40"/>
-    </row>
-    <row r="38" s="29" customFormat="1" spans="10:14">
-      <c r="J38" s="40"/>
-      <c r="N38" s="40"/>
-    </row>
-    <row r="39" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J39" s="40"/>
-      <c r="N39" s="40"/>
-    </row>
-    <row r="40" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J40" s="40"/>
-      <c r="N40" s="40"/>
-    </row>
-    <row r="41" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J41" s="40"/>
-      <c r="N41" s="40"/>
-    </row>
-    <row r="42" s="29" customFormat="1" customHeight="1" spans="10:14">
-      <c r="J42" s="40"/>
-      <c r="N42" s="40"/>
-    </row>
-    <row r="43" s="29" customFormat="1" spans="10:14">
-      <c r="J43" s="40"/>
-      <c r="N43" s="40"/>
-    </row>
-    <row r="44" s="29" customFormat="1" spans="10:14">
-      <c r="J44" s="40"/>
-      <c r="N44" s="40"/>
-    </row>
-    <row r="45" s="29" customFormat="1" spans="10:14">
-      <c r="J45" s="40"/>
-      <c r="N45" s="40"/>
-    </row>
-    <row r="46" s="29" customFormat="1" spans="10:14">
-      <c r="J46" s="40"/>
-      <c r="N46" s="40"/>
-    </row>
-    <row r="47" s="29" customFormat="1" spans="10:14">
-      <c r="J47" s="40"/>
-      <c r="N47" s="40"/>
-    </row>
-    <row r="48" s="29" customFormat="1" spans="10:14">
-      <c r="J48" s="40"/>
-      <c r="N48" s="40"/>
-    </row>
-    <row r="49" s="29" customFormat="1" spans="10:14">
-      <c r="J49" s="40"/>
-      <c r="N49" s="40"/>
-    </row>
-    <row r="50" s="29" customFormat="1" spans="10:14">
-      <c r="J50" s="40"/>
-      <c r="N50" s="40"/>
-    </row>
-    <row r="51" s="29" customFormat="1" spans="10:14">
-      <c r="J51" s="40"/>
-      <c r="N51" s="40"/>
-    </row>
-    <row r="52" s="29" customFormat="1" spans="10:14">
-      <c r="J52" s="40"/>
-      <c r="N52" s="40"/>
-    </row>
-    <row r="53" s="29" customFormat="1" spans="10:14">
-      <c r="J53" s="40"/>
-      <c r="N53" s="40"/>
-    </row>
-    <row r="54" s="29" customFormat="1" spans="10:14">
-      <c r="J54" s="40"/>
-      <c r="N54" s="40"/>
-    </row>
-    <row r="55" s="29" customFormat="1" spans="10:14">
-      <c r="J55" s="40"/>
-      <c r="N55" s="40"/>
+      <c r="J13" s="36"/>
+      <c r="N13" s="36"/>
+    </row>
+    <row r="14" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J14" s="35"/>
+      <c r="N14" s="35"/>
+    </row>
+    <row r="15" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J15" s="35"/>
+      <c r="N15" s="35"/>
+    </row>
+    <row r="16" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J16" s="35"/>
+      <c r="N16" s="35"/>
+    </row>
+    <row r="17" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J17" s="35"/>
+      <c r="N17" s="35"/>
+    </row>
+    <row r="18" s="24" customFormat="1" spans="10:14">
+      <c r="J18" s="35"/>
+      <c r="N18" s="35"/>
+    </row>
+    <row r="19" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J19" s="35"/>
+      <c r="N19" s="35"/>
+    </row>
+    <row r="20" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J20" s="35"/>
+      <c r="N20" s="35"/>
+    </row>
+    <row r="21" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J21" s="35"/>
+      <c r="N21" s="35"/>
+    </row>
+    <row r="22" s="24" customFormat="1" spans="10:14">
+      <c r="J22" s="35"/>
+      <c r="N22" s="35"/>
+    </row>
+    <row r="23" s="24" customFormat="1" spans="10:14">
+      <c r="J23" s="35"/>
+      <c r="N23" s="35"/>
+    </row>
+    <row r="24" s="24" customFormat="1" spans="10:14">
+      <c r="J24" s="35"/>
+      <c r="N24" s="35"/>
+    </row>
+    <row r="25" s="24" customFormat="1" ht="15.75" customHeight="1" spans="10:14">
+      <c r="J25" s="35"/>
+      <c r="N25" s="35"/>
+    </row>
+    <row r="26" s="24" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J26" s="35"/>
+      <c r="N26" s="35"/>
+    </row>
+    <row r="27" s="24" customFormat="1" spans="10:14">
+      <c r="J27" s="35"/>
+      <c r="N27" s="35"/>
+    </row>
+    <row r="28" s="24" customFormat="1" spans="10:14">
+      <c r="J28" s="35"/>
+      <c r="N28" s="35"/>
+    </row>
+    <row r="29" s="24" customFormat="1" spans="10:14">
+      <c r="J29" s="35"/>
+      <c r="N29" s="35"/>
+    </row>
+    <row r="30" s="24" customFormat="1" ht="13.5" customHeight="1" spans="10:14">
+      <c r="J30" s="35"/>
+      <c r="N30" s="35"/>
+    </row>
+    <row r="31" s="24" customFormat="1" spans="10:14">
+      <c r="J31" s="35"/>
+      <c r="N31" s="35"/>
+    </row>
+    <row r="32" s="24" customFormat="1" spans="10:14">
+      <c r="J32" s="35"/>
+      <c r="N32" s="35"/>
+    </row>
+    <row r="33" s="24" customFormat="1" spans="10:14">
+      <c r="J33" s="35"/>
+      <c r="N33" s="35"/>
+    </row>
+    <row r="34" s="24" customFormat="1" spans="10:14">
+      <c r="J34" s="35"/>
+      <c r="N34" s="35"/>
+    </row>
+    <row r="35" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J35" s="35"/>
+      <c r="N35" s="35"/>
+    </row>
+    <row r="36" s="24" customFormat="1" ht="12" customHeight="1" spans="10:14">
+      <c r="J36" s="35"/>
+      <c r="N36" s="35"/>
+    </row>
+    <row r="37" s="24" customFormat="1" spans="10:14">
+      <c r="J37" s="35"/>
+      <c r="N37" s="35"/>
+    </row>
+    <row r="38" s="24" customFormat="1" spans="10:14">
+      <c r="J38" s="35"/>
+      <c r="N38" s="35"/>
+    </row>
+    <row r="39" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J39" s="35"/>
+      <c r="N39" s="35"/>
+    </row>
+    <row r="40" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J40" s="35"/>
+      <c r="N40" s="35"/>
+    </row>
+    <row r="41" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J41" s="35"/>
+      <c r="N41" s="35"/>
+    </row>
+    <row r="42" s="24" customFormat="1" customHeight="1" spans="10:14">
+      <c r="J42" s="35"/>
+      <c r="N42" s="35"/>
+    </row>
+    <row r="43" s="24" customFormat="1" spans="10:14">
+      <c r="J43" s="35"/>
+      <c r="N43" s="35"/>
+    </row>
+    <row r="44" s="24" customFormat="1" spans="10:14">
+      <c r="J44" s="35"/>
+      <c r="N44" s="35"/>
+    </row>
+    <row r="45" s="24" customFormat="1" spans="10:14">
+      <c r="J45" s="35"/>
+      <c r="N45" s="35"/>
+    </row>
+    <row r="46" s="24" customFormat="1" spans="10:14">
+      <c r="J46" s="35"/>
+      <c r="N46" s="35"/>
+    </row>
+    <row r="47" s="24" customFormat="1" spans="10:14">
+      <c r="J47" s="35"/>
+      <c r="N47" s="35"/>
+    </row>
+    <row r="48" s="24" customFormat="1" spans="10:14">
+      <c r="J48" s="35"/>
+      <c r="N48" s="35"/>
+    </row>
+    <row r="49" s="24" customFormat="1" spans="10:14">
+      <c r="J49" s="35"/>
+      <c r="N49" s="35"/>
+    </row>
+    <row r="50" s="24" customFormat="1" spans="10:14">
+      <c r="J50" s="35"/>
+      <c r="N50" s="35"/>
+    </row>
+    <row r="51" s="24" customFormat="1" spans="10:14">
+      <c r="J51" s="35"/>
+      <c r="N51" s="35"/>
+    </row>
+    <row r="52" s="24" customFormat="1" spans="10:14">
+      <c r="J52" s="35"/>
+      <c r="N52" s="35"/>
+    </row>
+    <row r="53" s="24" customFormat="1" spans="10:14">
+      <c r="J53" s="35"/>
+      <c r="N53" s="35"/>
+    </row>
+    <row r="54" s="24" customFormat="1" spans="10:14">
+      <c r="J54" s="35"/>
+      <c r="N54" s="35"/>
+    </row>
+    <row r="55" s="24" customFormat="1" spans="10:14">
+      <c r="J55" s="35"/>
+      <c r="N55" s="35"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="29"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
-      <c r="I56" s="29"/>
-      <c r="J56" s="40"/>
-      <c r="K56" s="29"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2012,876 +1997,876 @@
       <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="13"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="13"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="13"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="13"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="14"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
       <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="6"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="19"/>
-      <c r="B54" s="19"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
       <c r="C54" s="6"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="19"/>
-      <c r="B55" s="19"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
       <c r="C55" s="6"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="19"/>
-      <c r="B56" s="19"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
       <c r="C56" s="6"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
       <c r="C57" s="6"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="19"/>
-      <c r="B58" s="19"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
       <c r="C58" s="6"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="19"/>
-      <c r="B59" s="19"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
       <c r="C59" s="6"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="19"/>
-      <c r="B60" s="19"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
       <c r="C60" s="6"/>
     </row>
     <row r="61" ht="15" spans="1:3">
-      <c r="A61" s="19"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="20"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" ht="15" spans="1:3">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="20"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
     </row>
     <row r="63" ht="15" spans="1:3">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="19"/>
-      <c r="B64" s="19"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
       <c r="C64" s="6"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="19"/>
-      <c r="B65" s="19"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="19"/>
-      <c r="B66" s="19"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
       <c r="C66" s="6"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="19"/>
-      <c r="B67" s="19"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
       <c r="C67" s="6"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="19"/>
-      <c r="B68" s="19"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="15"/>
       <c r="C68" s="6"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="19"/>
-      <c r="B69" s="19"/>
+      <c r="A69" s="15"/>
+      <c r="B69" s="15"/>
       <c r="C69" s="6"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="19"/>
-      <c r="B70" s="19"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="15"/>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="19"/>
-      <c r="B71" s="19"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="15"/>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="19"/>
-      <c r="B72" s="19"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="15"/>
       <c r="C72" s="6"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="19"/>
-      <c r="B73" s="19"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
       <c r="C73" s="6"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="19"/>
-      <c r="B74" s="19"/>
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
       <c r="C74" s="6"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="19"/>
-      <c r="B75" s="19"/>
+      <c r="A75" s="15"/>
+      <c r="B75" s="15"/>
       <c r="C75" s="6"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="19"/>
-      <c r="B76" s="19"/>
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
       <c r="C76" s="6"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="19"/>
-      <c r="B77" s="19"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="15"/>
       <c r="C77" s="6"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="19"/>
-      <c r="B78" s="19"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
       <c r="C78" s="6"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="19"/>
-      <c r="B79" s="19"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="15"/>
       <c r="C79" s="6"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="19"/>
-      <c r="B80" s="19"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="15"/>
       <c r="C80" s="6"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="19"/>
-      <c r="B81" s="19"/>
+      <c r="A81" s="15"/>
+      <c r="B81" s="15"/>
       <c r="C81" s="6"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="19"/>
-      <c r="B82" s="19"/>
+      <c r="A82" s="15"/>
+      <c r="B82" s="15"/>
       <c r="C82" s="6"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="19"/>
-      <c r="B83" s="19"/>
+      <c r="A83" s="15"/>
+      <c r="B83" s="15"/>
       <c r="C83" s="6"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="19"/>
-      <c r="B84" s="19"/>
+      <c r="A84" s="15"/>
+      <c r="B84" s="15"/>
       <c r="C84" s="6"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="19"/>
-      <c r="B85" s="19"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="15"/>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="19"/>
-      <c r="B86" s="19"/>
+      <c r="A86" s="15"/>
+      <c r="B86" s="15"/>
       <c r="C86" s="6"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="19"/>
-      <c r="B87" s="19"/>
+      <c r="A87" s="15"/>
+      <c r="B87" s="15"/>
       <c r="C87" s="6"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="19"/>
-      <c r="B88" s="19"/>
+      <c r="A88" s="15"/>
+      <c r="B88" s="15"/>
       <c r="C88" s="6"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="19"/>
-      <c r="B89" s="19"/>
+      <c r="A89" s="15"/>
+      <c r="B89" s="15"/>
       <c r="C89" s="6"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="19"/>
-      <c r="B90" s="19"/>
+      <c r="A90" s="15"/>
+      <c r="B90" s="15"/>
       <c r="C90" s="6"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="19"/>
-      <c r="B91" s="19"/>
+      <c r="A91" s="15"/>
+      <c r="B91" s="15"/>
       <c r="C91" s="6"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="19"/>
-      <c r="B92" s="19"/>
+      <c r="A92" s="15"/>
+      <c r="B92" s="15"/>
       <c r="C92" s="6"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="19"/>
-      <c r="B93" s="19"/>
+      <c r="A93" s="15"/>
+      <c r="B93" s="15"/>
       <c r="C93" s="6"/>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="19"/>
-      <c r="B94" s="19"/>
+      <c r="A94" s="15"/>
+      <c r="B94" s="15"/>
       <c r="C94" s="6"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="19"/>
-      <c r="B95" s="19"/>
+      <c r="A95" s="15"/>
+      <c r="B95" s="15"/>
       <c r="C95" s="6"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="19"/>
-      <c r="B96" s="19"/>
+      <c r="A96" s="15"/>
+      <c r="B96" s="15"/>
       <c r="C96" s="6"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="19"/>
-      <c r="B97" s="19"/>
+      <c r="A97" s="15"/>
+      <c r="B97" s="15"/>
       <c r="C97" s="6"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="19"/>
-      <c r="B98" s="19"/>
+      <c r="A98" s="15"/>
+      <c r="B98" s="15"/>
       <c r="C98" s="6"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="19"/>
-      <c r="B99" s="19"/>
+      <c r="A99" s="15"/>
+      <c r="B99" s="15"/>
       <c r="C99" s="6"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="19"/>
-      <c r="B100" s="19"/>
+      <c r="A100" s="15"/>
+      <c r="B100" s="15"/>
       <c r="C100" s="6"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="19"/>
-      <c r="B101" s="19"/>
+      <c r="A101" s="15"/>
+      <c r="B101" s="15"/>
       <c r="C101" s="6"/>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="19"/>
-      <c r="B102" s="19"/>
+      <c r="A102" s="15"/>
+      <c r="B102" s="15"/>
       <c r="C102" s="6"/>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="19"/>
-      <c r="B103" s="19"/>
+      <c r="A103" s="15"/>
+      <c r="B103" s="15"/>
       <c r="C103" s="6"/>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="19"/>
-      <c r="B104" s="19"/>
+      <c r="A104" s="15"/>
+      <c r="B104" s="15"/>
       <c r="C104" s="6"/>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="19"/>
-      <c r="B105" s="19"/>
+      <c r="A105" s="15"/>
+      <c r="B105" s="15"/>
       <c r="C105" s="6"/>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="19"/>
-      <c r="B106" s="19"/>
+      <c r="A106" s="15"/>
+      <c r="B106" s="15"/>
       <c r="C106" s="6"/>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="19"/>
-      <c r="B107" s="19"/>
+      <c r="A107" s="15"/>
+      <c r="B107" s="15"/>
       <c r="C107" s="6"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="19"/>
-      <c r="B108" s="19"/>
+      <c r="A108" s="15"/>
+      <c r="B108" s="15"/>
       <c r="C108" s="6"/>
-      <c r="D108" s="21"/>
+      <c r="D108" s="17"/>
       <c r="E108"/>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="19"/>
-      <c r="B109" s="19"/>
+      <c r="A109" s="15"/>
+      <c r="B109" s="15"/>
       <c r="C109" s="6"/>
-      <c r="D109" s="21"/>
+      <c r="D109" s="17"/>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="19"/>
-      <c r="B110" s="19"/>
+      <c r="A110" s="15"/>
+      <c r="B110" s="15"/>
       <c r="C110" s="6"/>
-      <c r="D110" s="21"/>
+      <c r="D110" s="17"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="19"/>
-      <c r="B111" s="19"/>
+      <c r="A111" s="15"/>
+      <c r="B111" s="15"/>
       <c r="C111" s="6"/>
-      <c r="D111" s="21"/>
+      <c r="D111" s="17"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="19"/>
-      <c r="B112" s="19"/>
+      <c r="A112" s="15"/>
+      <c r="B112" s="15"/>
       <c r="C112" s="6"/>
-      <c r="D112" s="21"/>
+      <c r="D112" s="17"/>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="19"/>
-      <c r="B113" s="19"/>
+      <c r="A113" s="15"/>
+      <c r="B113" s="15"/>
       <c r="C113" s="6"/>
-      <c r="D113" s="21"/>
+      <c r="D113" s="17"/>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="19"/>
-      <c r="B114" s="19"/>
+      <c r="A114" s="15"/>
+      <c r="B114" s="15"/>
       <c r="C114" s="6"/>
-      <c r="D114" s="21"/>
+      <c r="D114" s="17"/>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="19"/>
-      <c r="B115" s="19"/>
+      <c r="A115" s="15"/>
+      <c r="B115" s="15"/>
       <c r="C115" s="6"/>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="19"/>
-      <c r="B116" s="19"/>
+      <c r="A116" s="15"/>
+      <c r="B116" s="15"/>
       <c r="C116" s="6"/>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="19"/>
-      <c r="B117" s="19"/>
+      <c r="A117" s="15"/>
+      <c r="B117" s="15"/>
       <c r="C117" s="6"/>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="19"/>
-      <c r="B118" s="19"/>
+      <c r="A118" s="15"/>
+      <c r="B118" s="15"/>
       <c r="C118" s="6"/>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="19"/>
-      <c r="B119" s="19"/>
+      <c r="A119" s="15"/>
+      <c r="B119" s="15"/>
       <c r="C119" s="6"/>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="19"/>
-      <c r="B120" s="19"/>
+      <c r="A120" s="15"/>
+      <c r="B120" s="15"/>
       <c r="C120" s="6"/>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="19"/>
-      <c r="B121" s="19"/>
+      <c r="A121" s="15"/>
+      <c r="B121" s="15"/>
       <c r="C121" s="6"/>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="19"/>
-      <c r="B122" s="19"/>
+      <c r="A122" s="15"/>
+      <c r="B122" s="15"/>
       <c r="C122" s="6"/>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="19"/>
-      <c r="B123" s="19"/>
+      <c r="A123" s="15"/>
+      <c r="B123" s="15"/>
       <c r="C123" s="6"/>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="19"/>
-      <c r="B124" s="19"/>
+      <c r="A124" s="15"/>
+      <c r="B124" s="15"/>
       <c r="C124" s="6"/>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="19"/>
-      <c r="B125" s="19"/>
+      <c r="A125" s="15"/>
+      <c r="B125" s="15"/>
       <c r="C125" s="6"/>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="19"/>
-      <c r="B126" s="19"/>
+      <c r="A126" s="15"/>
+      <c r="B126" s="15"/>
       <c r="C126" s="6"/>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="19"/>
-      <c r="B127" s="19"/>
+      <c r="A127" s="15"/>
+      <c r="B127" s="15"/>
       <c r="C127" s="6"/>
     </row>
     <row r="128" spans="3:3">
-      <c r="C128" s="22"/>
+      <c r="C128" s="18"/>
     </row>
     <row r="129" spans="3:3">
-      <c r="C129" s="22"/>
+      <c r="C129" s="18"/>
     </row>
     <row r="130" spans="3:3">
-      <c r="C130" s="22"/>
+      <c r="C130" s="18"/>
     </row>
     <row r="131" spans="3:3">
-      <c r="C131" s="22"/>
+      <c r="C131" s="18"/>
     </row>
     <row r="132" spans="3:3">
-      <c r="C132" s="22"/>
+      <c r="C132" s="18"/>
     </row>
     <row r="133" spans="3:3">
-      <c r="C133" s="22"/>
+      <c r="C133" s="18"/>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" s="6"/>
     </row>
     <row r="135" spans="3:3">
-      <c r="C135" s="22"/>
+      <c r="C135" s="18"/>
     </row>
     <row r="136" spans="3:3">
-      <c r="C136" s="22"/>
+      <c r="C136" s="18"/>
     </row>
     <row r="137" spans="3:3">
-      <c r="C137" s="22"/>
+      <c r="C137" s="18"/>
     </row>
     <row r="138" spans="3:3">
-      <c r="C138" s="22"/>
+      <c r="C138" s="18"/>
     </row>
     <row r="139" spans="3:3">
-      <c r="C139" s="22"/>
+      <c r="C139" s="18"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="3"/>
-      <c r="C140" s="23"/>
+      <c r="C140" s="19"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="3"/>
-      <c r="C141" s="23"/>
+      <c r="C141" s="19"/>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="3"/>
-      <c r="C142" s="23"/>
+      <c r="C142" s="19"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="3"/>
-      <c r="C143" s="23"/>
+      <c r="C143" s="19"/>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="3"/>
-      <c r="C144" s="23"/>
+      <c r="C144" s="19"/>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="3"/>
-      <c r="C145" s="23"/>
+      <c r="C145" s="19"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="3"/>
-      <c r="C146" s="23"/>
+      <c r="C146" s="19"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="3"/>
-      <c r="C147" s="23"/>
+      <c r="C147" s="19"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="3"/>
-      <c r="C148" s="23"/>
+      <c r="C148" s="19"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="3"/>
-      <c r="C149" s="23"/>
+      <c r="C149" s="19"/>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="3"/>
-      <c r="C150" s="23"/>
+      <c r="C150" s="19"/>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="3"/>
-      <c r="C151" s="23"/>
+      <c r="C151" s="19"/>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="3"/>
-      <c r="C152" s="23"/>
+      <c r="C152" s="19"/>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="3"/>
-      <c r="C153" s="23"/>
+      <c r="C153" s="19"/>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="3"/>
-      <c r="C154" s="23"/>
+      <c r="C154" s="19"/>
     </row>
     <row r="155" spans="3:4">
-      <c r="C155" s="22"/>
-      <c r="D155" s="22"/>
+      <c r="C155" s="18"/>
+      <c r="D155" s="18"/>
     </row>
     <row r="156" spans="3:4">
-      <c r="C156" s="22"/>
-      <c r="D156" s="22"/>
+      <c r="C156" s="18"/>
+      <c r="D156" s="18"/>
     </row>
     <row r="157" spans="3:4">
-      <c r="C157" s="22"/>
-      <c r="D157" s="22"/>
+      <c r="C157" s="18"/>
+      <c r="D157" s="18"/>
     </row>
     <row r="158" spans="3:4">
-      <c r="C158" s="22"/>
-      <c r="D158" s="22"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="18"/>
     </row>
     <row r="159" spans="3:4">
-      <c r="C159" s="22"/>
-      <c r="D159" s="22"/>
+      <c r="C159" s="18"/>
+      <c r="D159" s="18"/>
     </row>
     <row r="160" spans="3:4">
-      <c r="C160" s="22"/>
-      <c r="D160" s="22"/>
+      <c r="C160" s="18"/>
+      <c r="D160" s="18"/>
     </row>
     <row r="161" spans="3:4">
-      <c r="C161" s="22"/>
-      <c r="D161" s="22"/>
+      <c r="C161" s="18"/>
+      <c r="D161" s="18"/>
     </row>
     <row r="162" spans="3:4">
-      <c r="C162" s="22"/>
-      <c r="D162" s="22"/>
+      <c r="C162" s="18"/>
+      <c r="D162" s="18"/>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="6"/>
       <c r="D163" s="6"/>
     </row>
     <row r="164" spans="3:3">
-      <c r="C164" s="22"/>
+      <c r="C164" s="18"/>
     </row>
     <row r="165" spans="3:3">
-      <c r="C165" s="22"/>
+      <c r="C165" s="18"/>
     </row>
     <row r="166" spans="3:3">
-      <c r="C166" s="22"/>
+      <c r="C166" s="18"/>
     </row>
     <row r="167" spans="3:3">
-      <c r="C167" s="22"/>
+      <c r="C167" s="18"/>
     </row>
     <row r="168" spans="3:3">
-      <c r="C168" s="22"/>
+      <c r="C168" s="18"/>
     </row>
     <row r="169" spans="3:3">
-      <c r="C169" s="22"/>
+      <c r="C169" s="18"/>
     </row>
     <row r="170" spans="3:3">
-      <c r="C170" s="22"/>
+      <c r="C170" s="18"/>
     </row>
     <row r="171" spans="3:3">
-      <c r="C171" s="22"/>
+      <c r="C171" s="18"/>
     </row>
     <row r="172" spans="3:3">
-      <c r="C172" s="22"/>
+      <c r="C172" s="18"/>
     </row>
     <row r="173" spans="3:3">
-      <c r="C173" s="22"/>
+      <c r="C173" s="18"/>
     </row>
     <row r="174" spans="3:3">
-      <c r="C174" s="22"/>
+      <c r="C174" s="18"/>
     </row>
     <row r="175" spans="3:3">
-      <c r="C175" s="22"/>
+      <c r="C175" s="18"/>
     </row>
     <row r="176" spans="3:3">
-      <c r="C176" s="22"/>
+      <c r="C176" s="18"/>
     </row>
     <row r="177" spans="3:3">
-      <c r="C177" s="22"/>
+      <c r="C177" s="18"/>
     </row>
     <row r="178" spans="3:3">
-      <c r="C178" s="22"/>
+      <c r="C178" s="18"/>
     </row>
     <row r="195" spans="3:3">
-      <c r="C195" s="22"/>
+      <c r="C195" s="18"/>
     </row>
     <row r="196" spans="3:3">
-      <c r="C196" s="22"/>
+      <c r="C196" s="18"/>
     </row>
     <row r="197" spans="3:3">
-      <c r="C197" s="22"/>
+      <c r="C197" s="18"/>
     </row>
     <row r="198" spans="3:3">
-      <c r="C198" s="22"/>
+      <c r="C198" s="18"/>
     </row>
     <row r="199" spans="3:3">
-      <c r="C199" s="22"/>
+      <c r="C199" s="18"/>
     </row>
     <row r="200" spans="3:3">
-      <c r="C200" s="22"/>
+      <c r="C200" s="18"/>
     </row>
     <row r="201" spans="3:3">
-      <c r="C201" s="22"/>
+      <c r="C201" s="18"/>
     </row>
     <row r="202" spans="3:3">
-      <c r="C202" s="22"/>
+      <c r="C202" s="18"/>
     </row>
     <row r="203" spans="3:3">
-      <c r="C203" s="22"/>
+      <c r="C203" s="18"/>
     </row>
     <row r="204" spans="3:3">
-      <c r="C204" s="22"/>
+      <c r="C204" s="18"/>
     </row>
     <row r="205" spans="3:3">
-      <c r="C205" s="22"/>
+      <c r="C205" s="18"/>
     </row>
     <row r="206" spans="3:3">
-      <c r="C206" s="22"/>
+      <c r="C206" s="18"/>
     </row>
     <row r="207" spans="3:3">
-      <c r="C207" s="22"/>
+      <c r="C207" s="18"/>
     </row>
     <row r="208" spans="3:3">
-      <c r="C208" s="22"/>
+      <c r="C208" s="18"/>
     </row>
     <row r="209" spans="3:3">
-      <c r="C209" s="22"/>
+      <c r="C209" s="18"/>
     </row>
     <row r="210" spans="3:3">
-      <c r="C210" s="22"/>
+      <c r="C210" s="18"/>
     </row>
     <row r="211" spans="3:3">
-      <c r="C211" s="22"/>
+      <c r="C211" s="18"/>
     </row>
     <row r="212" spans="3:3">
-      <c r="C212" s="22"/>
+      <c r="C212" s="18"/>
     </row>
     <row r="213" spans="3:3">
-      <c r="C213" s="22"/>
+      <c r="C213" s="18"/>
     </row>
     <row r="225" spans="3:3">
-      <c r="C225" s="24"/>
+      <c r="C225" s="20"/>
     </row>
     <row r="226" spans="3:3">
-      <c r="C226" s="24"/>
+      <c r="C226" s="20"/>
     </row>
     <row r="227" spans="3:3">
-      <c r="C227" s="25"/>
+      <c r="C227" s="21"/>
     </row>
     <row r="236" spans="3:3">
       <c r="C236" s="4"/>
@@ -2983,487 +2968,487 @@
       <c r="C268" s="4"/>
     </row>
     <row r="269" spans="3:3">
-      <c r="C269" s="21"/>
+      <c r="C269" s="17"/>
     </row>
     <row r="270" spans="3:3">
-      <c r="C270" s="21"/>
+      <c r="C270" s="17"/>
     </row>
     <row r="271" spans="3:3">
-      <c r="C271" s="21"/>
+      <c r="C271" s="17"/>
     </row>
     <row r="272" spans="3:3">
-      <c r="C272" s="21"/>
+      <c r="C272" s="17"/>
     </row>
     <row r="273" spans="3:3">
-      <c r="C273" s="21"/>
+      <c r="C273" s="17"/>
     </row>
     <row r="274" spans="3:3">
-      <c r="C274" s="21"/>
+      <c r="C274" s="17"/>
     </row>
     <row r="275" spans="3:3">
-      <c r="C275" s="21"/>
+      <c r="C275" s="17"/>
     </row>
     <row r="276" spans="3:3">
-      <c r="C276" s="21"/>
+      <c r="C276" s="17"/>
     </row>
     <row r="277" spans="3:3">
-      <c r="C277" s="21"/>
+      <c r="C277" s="17"/>
     </row>
     <row r="278" spans="3:3">
-      <c r="C278" s="21"/>
+      <c r="C278" s="17"/>
     </row>
     <row r="279" spans="3:3">
-      <c r="C279" s="21"/>
+      <c r="C279" s="17"/>
     </row>
     <row r="280" spans="3:3">
-      <c r="C280" s="21"/>
+      <c r="C280" s="17"/>
     </row>
     <row r="281" spans="3:3">
-      <c r="C281" s="21"/>
+      <c r="C281" s="17"/>
     </row>
     <row r="282" spans="3:3">
-      <c r="C282" s="21"/>
+      <c r="C282" s="17"/>
     </row>
     <row r="283" spans="3:3">
-      <c r="C283" s="21"/>
+      <c r="C283" s="17"/>
     </row>
     <row r="284" spans="3:3">
-      <c r="C284" s="21"/>
+      <c r="C284" s="17"/>
     </row>
     <row r="285" spans="3:3">
-      <c r="C285" s="21"/>
+      <c r="C285" s="17"/>
     </row>
     <row r="286" spans="3:3">
-      <c r="C286" s="21"/>
+      <c r="C286" s="17"/>
     </row>
     <row r="287" spans="3:3">
-      <c r="C287" s="21"/>
+      <c r="C287" s="17"/>
     </row>
     <row r="288" spans="3:3">
-      <c r="C288" s="21"/>
+      <c r="C288" s="17"/>
     </row>
     <row r="289" spans="3:3">
-      <c r="C289" s="21"/>
+      <c r="C289" s="17"/>
     </row>
     <row r="290" spans="3:3">
-      <c r="C290" s="21"/>
+      <c r="C290" s="17"/>
     </row>
     <row r="291" spans="3:3">
-      <c r="C291" s="21"/>
+      <c r="C291" s="17"/>
     </row>
     <row r="292" spans="3:3">
-      <c r="C292" s="21"/>
+      <c r="C292" s="17"/>
     </row>
     <row r="293" spans="3:3">
-      <c r="C293" s="21"/>
+      <c r="C293" s="17"/>
     </row>
     <row r="294" spans="3:3">
-      <c r="C294" s="21"/>
+      <c r="C294" s="17"/>
     </row>
     <row r="295" spans="3:3">
-      <c r="C295" s="21"/>
+      <c r="C295" s="17"/>
     </row>
     <row r="296" spans="3:3">
-      <c r="C296" s="21"/>
+      <c r="C296" s="17"/>
     </row>
     <row r="297" spans="3:3">
-      <c r="C297" s="21"/>
+      <c r="C297" s="17"/>
     </row>
     <row r="298" spans="3:3">
-      <c r="C298" s="21"/>
+      <c r="C298" s="17"/>
     </row>
     <row r="299" spans="3:3">
-      <c r="C299" s="21"/>
+      <c r="C299" s="17"/>
     </row>
     <row r="300" spans="3:3">
-      <c r="C300" s="21"/>
+      <c r="C300" s="17"/>
     </row>
     <row r="301" spans="3:3">
-      <c r="C301" s="21"/>
+      <c r="C301" s="17"/>
     </row>
     <row r="302" spans="3:3">
-      <c r="C302" s="21"/>
+      <c r="C302" s="17"/>
     </row>
     <row r="303" spans="3:3">
-      <c r="C303" s="21"/>
+      <c r="C303" s="17"/>
     </row>
     <row r="304" spans="3:3">
-      <c r="C304" s="21"/>
+      <c r="C304" s="17"/>
     </row>
     <row r="305" spans="3:3">
-      <c r="C305" s="21"/>
+      <c r="C305" s="17"/>
     </row>
     <row r="306" spans="3:3">
-      <c r="C306" s="21"/>
+      <c r="C306" s="17"/>
     </row>
     <row r="307" spans="3:3">
-      <c r="C307" s="21"/>
+      <c r="C307" s="17"/>
     </row>
     <row r="308" spans="3:3">
-      <c r="C308" s="21"/>
+      <c r="C308" s="17"/>
     </row>
     <row r="309" spans="3:3">
-      <c r="C309" s="21"/>
+      <c r="C309" s="17"/>
     </row>
     <row r="310" spans="3:3">
-      <c r="C310" s="21"/>
+      <c r="C310" s="17"/>
     </row>
     <row r="311" spans="3:3">
-      <c r="C311" s="21"/>
+      <c r="C311" s="17"/>
     </row>
     <row r="312" spans="3:3">
-      <c r="C312" s="21"/>
+      <c r="C312" s="17"/>
     </row>
     <row r="313" spans="3:3">
-      <c r="C313" s="21"/>
+      <c r="C313" s="17"/>
     </row>
     <row r="314" spans="3:3">
-      <c r="C314" s="21"/>
+      <c r="C314" s="17"/>
     </row>
     <row r="315" spans="3:3">
-      <c r="C315" s="21"/>
+      <c r="C315" s="17"/>
     </row>
     <row r="316" spans="3:3">
-      <c r="C316" s="21"/>
+      <c r="C316" s="17"/>
     </row>
     <row r="317" spans="3:3">
-      <c r="C317" s="21"/>
+      <c r="C317" s="17"/>
     </row>
     <row r="318" spans="3:3">
-      <c r="C318" s="21"/>
+      <c r="C318" s="17"/>
     </row>
     <row r="319" spans="3:3">
-      <c r="C319" s="21"/>
+      <c r="C319" s="17"/>
     </row>
     <row r="320" spans="3:3">
-      <c r="C320" s="21"/>
+      <c r="C320" s="17"/>
     </row>
     <row r="321" spans="3:3">
-      <c r="C321" s="21"/>
+      <c r="C321" s="17"/>
     </row>
     <row r="322" spans="3:3">
-      <c r="C322" s="21"/>
+      <c r="C322" s="17"/>
     </row>
     <row r="323" spans="3:3">
-      <c r="C323" s="21"/>
+      <c r="C323" s="17"/>
     </row>
     <row r="324" spans="3:3">
-      <c r="C324" s="21"/>
+      <c r="C324" s="17"/>
     </row>
     <row r="325" spans="3:3">
-      <c r="C325" s="21"/>
+      <c r="C325" s="17"/>
     </row>
     <row r="326" spans="3:3">
-      <c r="C326" s="21"/>
+      <c r="C326" s="17"/>
     </row>
     <row r="327" spans="3:3">
-      <c r="C327" s="21"/>
+      <c r="C327" s="17"/>
     </row>
     <row r="328" spans="3:3">
-      <c r="C328" s="21"/>
+      <c r="C328" s="17"/>
     </row>
     <row r="329" spans="3:3">
-      <c r="C329" s="21"/>
+      <c r="C329" s="17"/>
     </row>
     <row r="330" spans="3:3">
-      <c r="C330" s="21"/>
+      <c r="C330" s="17"/>
     </row>
     <row r="331" spans="3:3">
-      <c r="C331" s="21"/>
+      <c r="C331" s="17"/>
     </row>
     <row r="332" spans="3:3">
-      <c r="C332" s="21"/>
+      <c r="C332" s="17"/>
     </row>
     <row r="333" spans="3:3">
-      <c r="C333" s="21"/>
+      <c r="C333" s="17"/>
     </row>
     <row r="334" spans="3:3">
-      <c r="C334" s="21"/>
+      <c r="C334" s="17"/>
     </row>
     <row r="335" spans="3:3">
-      <c r="C335" s="21"/>
+      <c r="C335" s="17"/>
     </row>
     <row r="336" spans="3:3">
-      <c r="C336" s="21"/>
+      <c r="C336" s="17"/>
     </row>
     <row r="337" spans="3:3">
-      <c r="C337" s="21"/>
+      <c r="C337" s="17"/>
     </row>
     <row r="338" spans="3:3">
-      <c r="C338" s="21"/>
+      <c r="C338" s="17"/>
     </row>
     <row r="339" spans="3:3">
-      <c r="C339" s="21"/>
+      <c r="C339" s="17"/>
     </row>
     <row r="340" spans="3:3">
-      <c r="C340" s="21"/>
+      <c r="C340" s="17"/>
     </row>
     <row r="341" spans="3:3">
-      <c r="C341" s="21"/>
+      <c r="C341" s="17"/>
     </row>
     <row r="342" spans="3:3">
-      <c r="C342" s="21"/>
+      <c r="C342" s="17"/>
     </row>
     <row r="343" spans="3:3">
-      <c r="C343" s="21"/>
+      <c r="C343" s="17"/>
     </row>
     <row r="344" spans="3:3">
-      <c r="C344" s="21"/>
+      <c r="C344" s="17"/>
     </row>
     <row r="345" spans="3:3">
-      <c r="C345" s="21"/>
+      <c r="C345" s="17"/>
     </row>
     <row r="346" spans="3:3">
-      <c r="C346" s="21"/>
+      <c r="C346" s="17"/>
     </row>
     <row r="347" spans="3:3">
-      <c r="C347" s="21"/>
+      <c r="C347" s="17"/>
     </row>
     <row r="348" spans="3:3">
-      <c r="C348" s="21"/>
+      <c r="C348" s="17"/>
     </row>
     <row r="349" spans="3:3">
-      <c r="C349" s="21"/>
+      <c r="C349" s="17"/>
     </row>
     <row r="350" spans="3:3">
-      <c r="C350" s="21"/>
+      <c r="C350" s="17"/>
     </row>
     <row r="351" spans="3:3">
-      <c r="C351" s="21"/>
+      <c r="C351" s="17"/>
     </row>
     <row r="352" spans="3:3">
-      <c r="C352" s="21"/>
+      <c r="C352" s="17"/>
     </row>
     <row r="353" spans="3:3">
-      <c r="C353" s="21"/>
+      <c r="C353" s="17"/>
     </row>
     <row r="354" spans="3:3">
-      <c r="C354" s="21"/>
+      <c r="C354" s="17"/>
     </row>
     <row r="355" spans="3:3">
-      <c r="C355" s="21"/>
+      <c r="C355" s="17"/>
     </row>
     <row r="356" spans="3:3">
-      <c r="C356" s="21"/>
+      <c r="C356" s="17"/>
     </row>
     <row r="357" spans="3:3">
-      <c r="C357" s="21"/>
+      <c r="C357" s="17"/>
     </row>
     <row r="358" spans="3:3">
-      <c r="C358" s="21"/>
+      <c r="C358" s="17"/>
     </row>
     <row r="359" spans="3:3">
-      <c r="C359" s="21"/>
+      <c r="C359" s="17"/>
     </row>
     <row r="360" spans="3:3">
-      <c r="C360" s="21"/>
+      <c r="C360" s="17"/>
     </row>
     <row r="361" spans="3:3">
-      <c r="C361" s="21"/>
+      <c r="C361" s="17"/>
     </row>
     <row r="362" spans="3:3">
-      <c r="C362" s="21"/>
+      <c r="C362" s="17"/>
     </row>
     <row r="363" spans="3:3">
-      <c r="C363" s="21"/>
+      <c r="C363" s="17"/>
     </row>
     <row r="364" spans="3:3">
-      <c r="C364" s="21"/>
+      <c r="C364" s="17"/>
     </row>
     <row r="365" spans="3:3">
-      <c r="C365" s="21"/>
+      <c r="C365" s="17"/>
     </row>
     <row r="366" spans="3:3">
-      <c r="C366" s="21"/>
+      <c r="C366" s="17"/>
     </row>
     <row r="367" spans="3:3">
-      <c r="C367" s="21"/>
+      <c r="C367" s="17"/>
     </row>
     <row r="368" spans="3:3">
-      <c r="C368" s="21"/>
+      <c r="C368" s="17"/>
     </row>
     <row r="369" spans="3:3">
-      <c r="C369" s="21"/>
+      <c r="C369" s="17"/>
     </row>
     <row r="370" spans="3:3">
-      <c r="C370" s="21"/>
+      <c r="C370" s="17"/>
     </row>
     <row r="371" spans="3:3">
-      <c r="C371" s="21"/>
+      <c r="C371" s="17"/>
     </row>
     <row r="372" spans="3:3">
-      <c r="C372" s="21"/>
+      <c r="C372" s="17"/>
     </row>
     <row r="373" spans="3:3">
-      <c r="C373" s="21"/>
+      <c r="C373" s="17"/>
     </row>
     <row r="374" spans="3:3">
-      <c r="C374" s="21"/>
+      <c r="C374" s="17"/>
     </row>
     <row r="375" spans="3:3">
-      <c r="C375" s="21"/>
+      <c r="C375" s="17"/>
     </row>
     <row r="376" spans="3:3">
-      <c r="C376" s="21"/>
+      <c r="C376" s="17"/>
     </row>
     <row r="377" spans="3:3">
-      <c r="C377" s="21"/>
+      <c r="C377" s="17"/>
     </row>
     <row r="378" spans="3:3">
-      <c r="C378" s="21"/>
+      <c r="C378" s="17"/>
     </row>
     <row r="379" spans="3:3">
-      <c r="C379" s="21"/>
+      <c r="C379" s="17"/>
     </row>
     <row r="380" spans="3:3">
-      <c r="C380" s="21"/>
+      <c r="C380" s="17"/>
     </row>
     <row r="381" spans="3:3">
-      <c r="C381" s="21"/>
+      <c r="C381" s="17"/>
     </row>
     <row r="382" spans="3:3">
-      <c r="C382" s="21"/>
+      <c r="C382" s="17"/>
     </row>
     <row r="383" spans="3:3">
-      <c r="C383" s="21"/>
+      <c r="C383" s="17"/>
     </row>
     <row r="384" spans="3:3">
-      <c r="C384" s="21"/>
+      <c r="C384" s="17"/>
     </row>
     <row r="385" spans="3:3">
-      <c r="C385" s="21"/>
+      <c r="C385" s="17"/>
     </row>
     <row r="386" spans="3:3">
-      <c r="C386" s="21"/>
+      <c r="C386" s="17"/>
     </row>
     <row r="387" spans="3:3">
-      <c r="C387" s="21"/>
+      <c r="C387" s="17"/>
     </row>
     <row r="388" spans="3:3">
-      <c r="C388" s="21"/>
+      <c r="C388" s="17"/>
     </row>
     <row r="389" spans="3:3">
-      <c r="C389" s="21"/>
+      <c r="C389" s="17"/>
     </row>
     <row r="390" spans="3:3">
-      <c r="C390" s="21"/>
+      <c r="C390" s="17"/>
     </row>
     <row r="391" spans="3:3">
-      <c r="C391" s="21"/>
+      <c r="C391" s="17"/>
     </row>
     <row r="392" spans="3:3">
-      <c r="C392" s="21"/>
+      <c r="C392" s="17"/>
     </row>
     <row r="393" spans="3:3">
-      <c r="C393" s="21"/>
+      <c r="C393" s="17"/>
     </row>
     <row r="394" spans="3:3">
-      <c r="C394" s="21"/>
+      <c r="C394" s="17"/>
     </row>
     <row r="395" spans="3:3">
-      <c r="C395" s="21"/>
+      <c r="C395" s="17"/>
     </row>
     <row r="396" spans="3:3">
-      <c r="C396" s="21"/>
+      <c r="C396" s="17"/>
     </row>
     <row r="397" spans="3:3">
-      <c r="C397" s="21"/>
+      <c r="C397" s="17"/>
     </row>
     <row r="398" spans="3:3">
-      <c r="C398" s="21"/>
+      <c r="C398" s="17"/>
     </row>
     <row r="399" spans="3:3">
-      <c r="C399" s="21"/>
+      <c r="C399" s="17"/>
     </row>
     <row r="400" spans="3:3">
-      <c r="C400" s="21"/>
+      <c r="C400" s="17"/>
     </row>
     <row r="401" spans="3:3">
-      <c r="C401" s="21"/>
+      <c r="C401" s="17"/>
     </row>
     <row r="402" spans="3:3">
-      <c r="C402" s="21"/>
+      <c r="C402" s="17"/>
     </row>
     <row r="403" spans="3:3">
-      <c r="C403" s="21"/>
+      <c r="C403" s="17"/>
     </row>
     <row r="404" spans="3:3">
-      <c r="C404" s="21"/>
+      <c r="C404" s="17"/>
     </row>
     <row r="405" spans="3:3">
-      <c r="C405" s="21"/>
+      <c r="C405" s="17"/>
     </row>
     <row r="406" spans="3:3">
-      <c r="C406" s="21"/>
+      <c r="C406" s="17"/>
     </row>
     <row r="407" spans="3:3">
-      <c r="C407" s="21"/>
+      <c r="C407" s="17"/>
     </row>
     <row r="408" spans="3:3">
-      <c r="C408" s="21"/>
+      <c r="C408" s="17"/>
     </row>
     <row r="409" spans="3:3">
-      <c r="C409" s="21"/>
+      <c r="C409" s="17"/>
     </row>
     <row r="410" spans="3:3">
-      <c r="C410" s="21"/>
+      <c r="C410" s="17"/>
     </row>
     <row r="411" spans="3:3">
-      <c r="C411" s="21"/>
+      <c r="C411" s="17"/>
     </row>
     <row r="412" spans="3:3">
-      <c r="C412" s="21"/>
+      <c r="C412" s="17"/>
     </row>
     <row r="413" spans="3:3">
-      <c r="C413" s="21"/>
+      <c r="C413" s="17"/>
     </row>
     <row r="414" spans="3:3">
-      <c r="C414" s="21"/>
+      <c r="C414" s="17"/>
     </row>
     <row r="415" spans="3:3">
-      <c r="C415" s="21"/>
+      <c r="C415" s="17"/>
     </row>
     <row r="416" spans="3:3">
-      <c r="C416" s="21"/>
+      <c r="C416" s="17"/>
     </row>
     <row r="417" spans="3:3">
-      <c r="C417" s="21"/>
+      <c r="C417" s="17"/>
     </row>
     <row r="418" spans="3:3">
-      <c r="C418" s="21"/>
+      <c r="C418" s="17"/>
     </row>
     <row r="419" spans="3:3">
-      <c r="C419" s="21"/>
+      <c r="C419" s="17"/>
     </row>
     <row r="420" spans="3:3">
-      <c r="C420" s="21"/>
+      <c r="C420" s="17"/>
     </row>
     <row r="421" spans="3:3">
-      <c r="C421" s="21"/>
+      <c r="C421" s="17"/>
     </row>
     <row r="422" spans="3:3">
-      <c r="C422" s="21"/>
+      <c r="C422" s="17"/>
     </row>
     <row r="423" spans="3:3">
-      <c r="C423" s="21"/>
+      <c r="C423" s="17"/>
     </row>
     <row r="424" spans="3:3">
-      <c r="C424" s="21"/>
+      <c r="C424" s="17"/>
     </row>
     <row r="425" spans="3:3">
-      <c r="C425" s="21"/>
+      <c r="C425" s="17"/>
     </row>
     <row r="426" spans="3:3">
-      <c r="C426" s="21"/>
+      <c r="C426" s="17"/>
     </row>
     <row r="434" spans="3:3">
-      <c r="C434" s="26"/>
+      <c r="C434" s="22"/>
     </row>
     <row r="435" spans="3:3">
-      <c r="C435" s="26"/>
+      <c r="C435" s="22"/>
     </row>
     <row r="436" spans="3:3">
-      <c r="C436" s="26"/>
+      <c r="C436" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3477,8 +3462,8 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.54166666666667" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="2" outlineLevelCol="4"/>

</xml_diff>